<commit_message>
new milk peptides benchmark complete
</commit_message>
<xml_diff>
--- a/benchmarking/milk-allergens-benchmarking.xlsx
+++ b/benchmarking/milk-allergens-benchmarking.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">N/A</t>
   </si>
   <si>
-    <t xml:space="preserve">NmerMatch</t>
+    <t xml:space="preserve">NmerMatch (J Greenbaum)</t>
   </si>
   <si>
     <t xml:space="preserve">BLAST</t>
@@ -162,7 +162,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -224,118 +224,118 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>46.247</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>193.638</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>239.885</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="3" t="n">
+      <c r="B2" s="0" t="n">
+        <v>45.488312</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>600.325347</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>645.813659</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="n">
-        <v>51.734304</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>0.003208</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>242.395365</v>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>294.132877</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="3" t="n">
+      <c r="B3" s="0" t="n">
+        <v>203.719</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.00473928451538086</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1168.358</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1372.082</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="0" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>1.329</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>16.628</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>17.958</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>31.25</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="B4" s="0" t="n">
+        <v>1.301</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>105.282</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>106.583</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>84.195</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>0.239</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>4.773</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>5.012</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>19.432</v>
+      <c r="B5" s="0" t="n">
+        <v>0.249</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>5.238</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>5.487</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>75.332</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>2.726</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>0.438</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>3.163</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>22.273</v>
+      <c r="B6" s="0" t="n">
+        <v>2.253</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0.484</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>2.737</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>75.628</v>
       </c>
     </row>
   </sheetData>

</xml_diff>